<commit_message>
Adding some small changes
For fixing excel report.
For adding build year and type to items.
</commit_message>
<xml_diff>
--- a/eFormAPI/Plugins/ItemsPlanning.Pn/ItemsPlanning.Pn/Resources/Templates/report_template.xlsx
+++ b/eFormAPI/Plugins/ItemsPlanning.Pn/ItemsPlanning.Pn/Resources/Templates/report_template.xlsx
@@ -1,41 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -47,358 +66,127 @@
     </fill>
   </fills>
   <borders count="2">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
-  <a:themeElements>
-    <a:clrScheme name="Стандартная">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Стандартная">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A2:AH41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.53"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B2" s="2"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -434,7 +222,7 @@
       <c r="AG7" s="5"/>
       <c r="AH7" s="5"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -470,7 +258,7 @@
       <c r="AG8" s="5"/>
       <c r="AH8" s="5"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -506,7 +294,7 @@
       <c r="AG9" s="5"/>
       <c r="AH9" s="5"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -542,7 +330,7 @@
       <c r="AG10" s="5"/>
       <c r="AH10" s="5"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -578,7 +366,7 @@
       <c r="AG11" s="5"/>
       <c r="AH11" s="5"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -614,7 +402,7 @@
       <c r="AG12" s="5"/>
       <c r="AH12" s="5"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -650,7 +438,7 @@
       <c r="AG13" s="5"/>
       <c r="AH13" s="5"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -686,7 +474,7 @@
       <c r="AG14" s="5"/>
       <c r="AH14" s="5"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -722,7 +510,7 @@
       <c r="AG15" s="5"/>
       <c r="AH15" s="5"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -758,7 +546,7 @@
       <c r="AG16" s="5"/>
       <c r="AH16" s="5"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -794,7 +582,7 @@
       <c r="AG17" s="5"/>
       <c r="AH17" s="5"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -830,7 +618,7 @@
       <c r="AG18" s="5"/>
       <c r="AH18" s="5"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -866,7 +654,7 @@
       <c r="AG19" s="5"/>
       <c r="AH19" s="5"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -902,7 +690,7 @@
       <c r="AG20" s="5"/>
       <c r="AH20" s="5"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -938,7 +726,7 @@
       <c r="AG21" s="5"/>
       <c r="AH21" s="5"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -974,7 +762,7 @@
       <c r="AG22" s="5"/>
       <c r="AH22" s="5"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1010,7 +798,7 @@
       <c r="AG23" s="5"/>
       <c r="AH23" s="5"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1046,7 +834,7 @@
       <c r="AG24" s="5"/>
       <c r="AH24" s="5"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1082,7 +870,7 @@
       <c r="AG25" s="5"/>
       <c r="AH25" s="5"/>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1118,7 +906,7 @@
       <c r="AG26" s="5"/>
       <c r="AH26" s="5"/>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1154,7 +942,7 @@
       <c r="AG27" s="5"/>
       <c r="AH27" s="5"/>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1190,7 +978,7 @@
       <c r="AG28" s="5"/>
       <c r="AH28" s="5"/>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1226,7 +1014,7 @@
       <c r="AG29" s="5"/>
       <c r="AH29" s="5"/>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1262,7 +1050,7 @@
       <c r="AG30" s="5"/>
       <c r="AH30" s="5"/>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1298,7 +1086,7 @@
       <c r="AG31" s="5"/>
       <c r="AH31" s="5"/>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1334,7 +1122,7 @@
       <c r="AG32" s="5"/>
       <c r="AH32" s="5"/>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1370,7 +1158,7 @@
       <c r="AG33" s="5"/>
       <c r="AH33" s="5"/>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1406,7 +1194,7 @@
       <c r="AG34" s="5"/>
       <c r="AH34" s="5"/>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1442,7 +1230,7 @@
       <c r="AG35" s="5"/>
       <c r="AH35" s="5"/>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1478,7 +1266,7 @@
       <c r="AG36" s="5"/>
       <c r="AH36" s="5"/>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1514,7 +1302,7 @@
       <c r="AG37" s="5"/>
       <c r="AH37" s="5"/>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1550,7 +1338,7 @@
       <c r="AG38" s="5"/>
       <c r="AH38" s="5"/>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1586,7 +1374,7 @@
       <c r="AG39" s="5"/>
       <c r="AH39" s="5"/>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1622,7 +1410,7 @@
       <c r="AG40" s="5"/>
       <c r="AH40" s="5"/>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1659,7 +1447,12 @@
       <c r="AH41" s="5"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>